<commit_message>
Rewrote README, added example file, removed unnecessary files, fixed main.py: reordered imports, added a functionality to indicate the location of file instead of only its name
</commit_message>
<xml_diff>
--- a/wine.xlsx
+++ b/wine.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOSBAIGUT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jticorp-my.sharepoint.com/personal/mosbaigut_corp_jti_com/Documents/Desktop/wine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1518E3-2A8A-4236-88F6-D27679D0A116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{566FF987-1D27-442F-960E-0F01419BFBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Название</t>
   </si>
@@ -34,27 +34,6 @@
     <t>Картинка</t>
   </si>
   <si>
-    <t>Изабелла</t>
-  </si>
-  <si>
-    <t>izabella.png</t>
-  </si>
-  <si>
-    <t>Гранатовый браслет</t>
-  </si>
-  <si>
-    <t>Мускат розовый</t>
-  </si>
-  <si>
-    <t>granatovyi_braslet.png</t>
-  </si>
-  <si>
-    <t>Шардоне</t>
-  </si>
-  <si>
-    <t>shardone.png</t>
-  </si>
-  <si>
     <t>Белая леди</t>
   </si>
   <si>
@@ -77,13 +56,73 @@
   </si>
   <si>
     <t>hvanchkara.png</t>
+  </si>
+  <si>
+    <t>Категория</t>
+  </si>
+  <si>
+    <t>Белые вина</t>
+  </si>
+  <si>
+    <t>Напитки</t>
+  </si>
+  <si>
+    <t>Коньяк классический</t>
+  </si>
+  <si>
+    <t>konyak_klassicheskyi.png</t>
+  </si>
+  <si>
+    <t>Красные вина</t>
+  </si>
+  <si>
+    <t>Черный лекарь</t>
+  </si>
+  <si>
+    <t>Качич</t>
+  </si>
+  <si>
+    <t>chernyi_lekar.png</t>
+  </si>
+  <si>
+    <t>Кокур</t>
+  </si>
+  <si>
+    <t>kokur.png</t>
+  </si>
+  <si>
+    <t>Киндзмараули</t>
+  </si>
+  <si>
+    <t>Саперави</t>
+  </si>
+  <si>
+    <t>kindzmarauli.png</t>
+  </si>
+  <si>
+    <t>Чача</t>
+  </si>
+  <si>
+    <t>chacha.png</t>
+  </si>
+  <si>
+    <t>Коньяк кизиловый</t>
+  </si>
+  <si>
+    <t>konyak_kizilovyi.png</t>
+  </si>
+  <si>
+    <t>Акция</t>
+  </si>
+  <si>
+    <t>Выгодное предложение</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,11 +133,24 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,15 +173,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,116 +403,204 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>399</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4">
         <v>350</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4">
+        <v>499</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4">
+        <v>399</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4">
+        <v>550</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4">
+        <v>450</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4">
+        <v>550</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4">
+        <v>299</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4">
         <v>350</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2">
-        <v>350</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
-        <v>399</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2">
-        <v>499</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2">
-        <v>550</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>